<commit_message>
added automatic switch to google scraper
</commit_message>
<xml_diff>
--- a/Shopee Test.xlsx
+++ b/Shopee Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jabezlee/Desktop/Capstone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylan/Desktop/Y4S1/BT4103/Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD006DB-F260-D34C-BB4A-81CA7A41D07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8A2C7D-B041-D245-A2F7-F28D7A374656}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="-21000" windowWidth="28800" windowHeight="16520" xr2:uid="{96BD78DB-808C-4DC5-B7D6-F07A8C9CF258}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{96BD78DB-808C-4DC5-B7D6-F07A8C9CF258}"/>
   </bookViews>
   <sheets>
     <sheet name="Individuals" sheetId="1" r:id="rId1"/>
@@ -20,26 +20,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Corporates!$A$1:$C$142</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Individuals!$A$1:$G$7</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="184">
   <si>
     <t>Name to be screened</t>
   </si>
@@ -108,9 +99,6 @@
   </si>
   <si>
     <t>Son Mun San</t>
-  </si>
-  <si>
-    <t>Son Mnu San</t>
   </si>
   <si>
     <t>Male</t>
@@ -1099,7 +1087,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1146,10 +1134,10 @@
         <v>1977</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>7</v>
@@ -1167,10 +1155,10 @@
         <v>22304</v>
       </c>
       <c r="D3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>12</v>
@@ -1188,7 +1176,7 @@
         <v>25061</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>16</v>
@@ -1209,10 +1197,10 @@
         <v>1987</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>7</v>
@@ -1228,10 +1216,10 @@
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>8</v>
@@ -1242,7 +1230,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15">
@@ -1261,44 +1249,44 @@
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17">
         <v>1997</v>
       </c>
       <c r="D9" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="17"/>
@@ -1345,1553 +1333,1553 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B54" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="C54" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C85" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C87" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C88" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C89" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C90" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="28" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B101" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B102" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B103" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B105" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B107" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B110" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B112" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B113" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B116" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C117" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="B117" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B118" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B120" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B122" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B123" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B126" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C128" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="B128" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C128" s="8" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B129" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B130" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B131" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B132" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B133" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B135" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B137" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B138" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B140" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B141" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>